<commit_message>
Calibration Curves Generated for Pressure
</commit_message>
<xml_diff>
--- a/analysis/Pressure Calibration/100psi.xlsx
+++ b/analysis/Pressure Calibration/100psi.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam-n-Abbs\Documents\GitHub\liquid-engine-test-stand\analysis\Pressure Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E6ACAAA-A9E1-464B-B4DC-2BF66503D884}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB2BCE-028E-499C-A180-BD085DA65B57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="9345"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="9345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Data" sheetId="1" r:id="rId1"/>
     <sheet name="Simple Data with Plots" sheetId="4" r:id="rId2"/>
     <sheet name="Interactive Bar Graph" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="92512"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
   <si>
     <t>Move this sheet to 1st tab position to accept data</t>
   </si>
@@ -90,11 +90,26 @@
   <si>
     <t xml:space="preserve"> 5:09:01 PM</t>
   </si>
+  <si>
+    <t>avg1</t>
+  </si>
+  <si>
+    <t>avg2</t>
+  </si>
+  <si>
+    <t>avg3</t>
+  </si>
+  <si>
+    <t>avg4</t>
+  </si>
+  <si>
+    <t>avg5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1416,12 +1431,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1448,7 @@
     <col min="7" max="10" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1476,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1486,8 +1501,15 @@
       <c r="H2" s="1">
         <v>896</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <f>D2:D66</f>
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
@@ -1512,8 +1534,15 @@
       <c r="H3" s="1">
         <v>888</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(E2:E66)</f>
+        <v>406.32307692307694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1538,8 +1567,15 @@
       <c r="H4" s="1">
         <v>894</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(F2:F66)</f>
+        <v>973.93846153846152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -1564,8 +1600,15 @@
       <c r="H5" s="1">
         <v>899</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(G2:G66)</f>
+        <v>337.12307692307695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1590,8 +1633,15 @@
       <c r="H6" s="1">
         <v>901</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(H2:H66)</f>
+        <v>895.89230769230767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -1617,7 +1667,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
@@ -1643,7 +1693,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1669,7 +1719,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1745,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1771,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1747,7 +1797,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
@@ -1773,7 +1823,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -1799,7 +1849,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
@@ -1825,7 +1875,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -3159,7 +3209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -3209,7 +3259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E8"/>
   <sheetViews>

</xml_diff>